<commit_message>
updates minor incl kelp counts curation
</commit_message>
<xml_diff>
--- a/curation/kelp_counts_curated.xlsx
+++ b/curation/kelp_counts_curated.xlsx
@@ -390,10 +390,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2016</t>
-        </is>
+      <c r="A2">
+        <v>17</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -410,10 +408,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2017</t>
-        </is>
+      <c r="A3">
+        <v>18</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -430,10 +426,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2018</t>
-        </is>
+      <c r="A4">
+        <v>19</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -485,10 +479,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2016</t>
-        </is>
+      <c r="A2">
+        <v>17</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -505,10 +497,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2017</t>
-        </is>
+      <c r="A3">
+        <v>18</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -525,10 +515,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2018</t>
-        </is>
+      <c r="A4">
+        <v>19</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -580,10 +568,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2016</t>
-        </is>
+      <c r="A2">
+        <v>17</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -600,10 +586,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2017</t>
-        </is>
+      <c r="A3">
+        <v>18</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -620,10 +604,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2018</t>
-        </is>
+      <c r="A4">
+        <v>19</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -675,10 +657,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2016</t>
-        </is>
+      <c r="A2">
+        <v>17</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -695,10 +675,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2017</t>
-        </is>
+      <c r="A3">
+        <v>18</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -715,10 +693,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2018</t>
-        </is>
+      <c r="A4">
+        <v>19</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -770,10 +746,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2016</t>
-        </is>
+      <c r="A2">
+        <v>17</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -790,10 +764,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2017</t>
-        </is>
+      <c r="A3">
+        <v>18</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -810,10 +782,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2018</t>
-        </is>
+      <c r="A4">
+        <v>19</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -865,10 +835,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2016</t>
-        </is>
+      <c r="A2">
+        <v>17</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -885,10 +853,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2017</t>
-        </is>
+      <c r="A3">
+        <v>18</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -940,10 +906,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2016</t>
-        </is>
+      <c r="A2">
+        <v>17</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -960,10 +924,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2017</t>
-        </is>
+      <c r="A3">
+        <v>18</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -980,10 +942,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2018</t>
-        </is>
+      <c r="A4">
+        <v>19</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -1035,10 +995,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2016</t>
-        </is>
+      <c r="A2">
+        <v>17</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -1055,10 +1013,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2017</t>
-        </is>
+      <c r="A3">
+        <v>18</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -1075,10 +1031,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2018</t>
-        </is>
+      <c r="A4">
+        <v>19</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -1130,10 +1084,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2016</t>
-        </is>
+      <c r="A2">
+        <v>17</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -1150,10 +1102,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2017</t>
-        </is>
+      <c r="A3">
+        <v>18</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -1170,10 +1120,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2018</t>
-        </is>
+      <c r="A4">
+        <v>19</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -1225,10 +1173,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2016</t>
-        </is>
+      <c r="A2">
+        <v>17</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -1245,10 +1191,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2017</t>
-        </is>
+      <c r="A3">
+        <v>18</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -1265,10 +1209,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2018</t>
-        </is>
+      <c r="A4">
+        <v>19</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -1320,10 +1262,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2016</t>
-        </is>
+      <c r="A2">
+        <v>17</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -1340,10 +1280,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2017</t>
-        </is>
+      <c r="A3">
+        <v>18</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -1360,10 +1298,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2018</t>
-        </is>
+      <c r="A4">
+        <v>19</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>

</xml_diff>